<commit_message>
add bootstrap table plugin
</commit_message>
<xml_diff>
--- a/src/main/resources/templet/download/addready.xlsx
+++ b/src/main/resources/templet/download/addready.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>客户</t>
   </si>
@@ -90,31 +90,142 @@
     <t>折扣后金额</t>
   </si>
   <si>
-    <t>入库时间</t>
-  </si>
-  <si>
-    <t>入库数量</t>
-  </si>
-  <si>
     <t>检测时间</t>
   </si>
   <si>
     <t>检测结果</t>
   </si>
   <si>
-    <t>出库时间</t>
-  </si>
-  <si>
-    <t>出库数量</t>
-  </si>
-  <si>
-    <t>挂账数量</t>
-  </si>
-  <si>
-    <t>挂账金额</t>
-  </si>
-  <si>
-    <t>挂账日期</t>
+    <t>入库时间1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入库数量1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入库数量2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入库时间2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入库时间3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入库数量3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入库时间5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入库数量5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库时间1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库数量2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库时间3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库数量3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库时间4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库数量4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库时间5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库数量5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账数量1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账金额1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账日期1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账数量2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账金额2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账日期2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账数量3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账金额3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账日期3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账数量4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账金额4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账日期4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账数量5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账金额5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挂账日期5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库数量1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出库时间2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -153,7 +264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -176,13 +287,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -192,6 +316,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -493,15 +621,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:BI1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AI1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="6" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.125" customWidth="1"/>
+    <col min="30" max="30" width="12.75" customWidth="1"/>
+    <col min="31" max="31" width="12.125" customWidth="1"/>
+    <col min="32" max="32" width="12.25" customWidth="1"/>
+    <col min="33" max="33" width="12.875" customWidth="1"/>
+    <col min="34" max="34" width="11.125" customWidth="1"/>
+    <col min="35" max="35" width="11.875" customWidth="1"/>
+    <col min="36" max="36" width="11.5" customWidth="1"/>
+    <col min="37" max="37" width="14.625" customWidth="1"/>
+    <col min="38" max="38" width="12.25" customWidth="1"/>
+    <col min="39" max="41" width="11.5" customWidth="1"/>
+    <col min="42" max="42" width="10.375" customWidth="1"/>
+    <col min="43" max="43" width="10.875" customWidth="1"/>
+    <col min="44" max="44" width="11.125" customWidth="1"/>
+    <col min="45" max="45" width="11" customWidth="1"/>
+    <col min="46" max="46" width="10" customWidth="1"/>
+    <col min="47" max="47" width="14.25" customWidth="1"/>
+    <col min="48" max="48" width="10.5" customWidth="1"/>
+    <col min="49" max="49" width="10.125" customWidth="1"/>
+    <col min="50" max="50" width="10.5" customWidth="1"/>
+    <col min="51" max="51" width="13.375" customWidth="1"/>
+    <col min="52" max="52" width="12.375" customWidth="1"/>
+    <col min="53" max="53" width="10.5" customWidth="1"/>
+    <col min="54" max="54" width="10.25" customWidth="1"/>
+    <col min="55" max="55" width="11.625" customWidth="1"/>
+    <col min="56" max="56" width="10.75" customWidth="1"/>
+    <col min="57" max="57" width="9.5" customWidth="1"/>
+    <col min="58" max="58" width="10.875" customWidth="1"/>
+    <col min="59" max="60" width="11.5" customWidth="1"/>
+    <col min="61" max="61" width="12.25" customWidth="1"/>
+    <col min="62" max="62" width="11" customWidth="1"/>
+    <col min="63" max="63" width="11.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="27">
+    <row r="1" spans="1:61" s="4" customFormat="1" ht="27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,10 +757,10 @@
         <v>27</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>30</v>
@@ -606,6 +770,84 @@
       </c>
       <c r="AI1" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>